<commit_message>
Complete IEP Graph and Upload Updates 2023-2024 dataset
</commit_message>
<xml_diff>
--- a/data/ignore/2023-2024.xlsx
+++ b/data/ignore/2023-2024.xlsx
@@ -741,7 +741,7 @@
         <v>10.0</v>
       </c>
       <c r="F14" s="7">
-        <f>E14/B14*100</f>
+        <f t="shared" ref="F14:F15" si="3">E14/B14*100</f>
         <v>43.47826087</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -766,8 +766,8 @@
         <v>72</v>
       </c>
       <c r="F15" s="7">
-        <f>E14/B15*100</f>
-        <v>11.11111111</v>
+        <f t="shared" si="3"/>
+        <v>80</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>10</v>
@@ -813,7 +813,7 @@
         <v>9.0</v>
       </c>
       <c r="F17" s="7">
-        <f t="shared" ref="F17:F22" si="3">E17/B17*100</f>
+        <f t="shared" ref="F17:F22" si="4">E17/B17*100</f>
         <v>81.81818182</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -837,7 +837,7 @@
         <v>16.0</v>
       </c>
       <c r="F18" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>59.25925926</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -861,7 +861,7 @@
         <v>3.0</v>
       </c>
       <c r="F19" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.07692308</v>
       </c>
       <c r="G19" s="4" t="s">
@@ -885,7 +885,7 @@
         <v>25.0</v>
       </c>
       <c r="F20" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.33333333</v>
       </c>
       <c r="G20" s="4" t="s">
@@ -909,7 +909,7 @@
         <v>7.0</v>
       </c>
       <c r="F21" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30.43478261</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -934,7 +934,7 @@
         <v>60</v>
       </c>
       <c r="F22" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67.41573034</v>
       </c>
       <c r="G22" s="4" t="s">
@@ -981,7 +981,7 @@
         <v>11.0</v>
       </c>
       <c r="F24" s="7">
-        <f t="shared" ref="F24:F29" si="4">E24/B24*100</f>
+        <f t="shared" ref="F24:F29" si="5">E24/B24*100</f>
         <v>100</v>
       </c>
       <c r="G24" s="4" t="s">
@@ -1005,7 +1005,7 @@
         <v>22.0</v>
       </c>
       <c r="F25" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>81.48148148</v>
       </c>
       <c r="G25" s="4" t="s">
@@ -1029,7 +1029,7 @@
         <v>5.0</v>
       </c>
       <c r="F26" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>38.46153846</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -1053,7 +1053,7 @@
         <v>24.0</v>
       </c>
       <c r="F27" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>80</v>
       </c>
       <c r="G27" s="4" t="s">
@@ -1077,7 +1077,7 @@
         <v>7.0</v>
       </c>
       <c r="F28" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30.43478261</v>
       </c>
       <c r="G28" s="4" t="s">
@@ -1101,7 +1101,7 @@
         <v>65.0</v>
       </c>
       <c r="F29" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.03370787</v>
       </c>
       <c r="G29" s="4" t="s">
@@ -1148,7 +1148,7 @@
         <v>11.0</v>
       </c>
       <c r="F31" s="7">
-        <f t="shared" ref="F31:F36" si="5">E31/B31*100</f>
+        <f t="shared" ref="F31:F36" si="6">E31/B31*100</f>
         <v>100</v>
       </c>
       <c r="G31" s="4" t="s">
@@ -1172,7 +1172,7 @@
         <v>17.0</v>
       </c>
       <c r="F32" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62.96296296</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -1196,7 +1196,7 @@
         <v>2.0</v>
       </c>
       <c r="F33" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16.66666667</v>
       </c>
       <c r="G33" s="4" t="s">
@@ -1220,7 +1220,7 @@
         <v>21.0</v>
       </c>
       <c r="F34" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>70</v>
       </c>
       <c r="G34" s="4" t="s">
@@ -1244,7 +1244,7 @@
         <v>10.0</v>
       </c>
       <c r="F35" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>45.45454545</v>
       </c>
       <c r="G35" s="4" t="s">
@@ -1268,7 +1268,7 @@
         <v>65.0</v>
       </c>
       <c r="F36" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>73.86363636</v>
       </c>
       <c r="G36" s="4" t="s">
@@ -1315,7 +1315,7 @@
         <v>10.0</v>
       </c>
       <c r="F38" s="7">
-        <f t="shared" ref="F38:F43" si="6">E38/B38*100</f>
+        <f t="shared" ref="F38:F43" si="7">E38/B38*100</f>
         <v>90.90909091</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -1339,7 +1339,7 @@
         <v>21.0</v>
       </c>
       <c r="F39" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>77.77777778</v>
       </c>
       <c r="G39" s="4" t="s">
@@ -1363,7 +1363,7 @@
         <v>4.0</v>
       </c>
       <c r="F40" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33.33333333</v>
       </c>
       <c r="G40" s="4" t="s">
@@ -1387,7 +1387,7 @@
         <v>24.0</v>
       </c>
       <c r="F41" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>80</v>
       </c>
       <c r="G41" s="4" t="s">
@@ -1411,7 +1411,7 @@
         <v>5.0</v>
       </c>
       <c r="F42" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>23.80952381</v>
       </c>
       <c r="G42" s="4" t="s">
@@ -1435,7 +1435,7 @@
         <v>44.0</v>
       </c>
       <c r="F43" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>50.57471264</v>
       </c>
       <c r="G43" s="4" t="s">
@@ -1482,7 +1482,7 @@
         <v>11.0</v>
       </c>
       <c r="F45" s="7">
-        <f t="shared" ref="F45:F50" si="7">E45/B45*100</f>
+        <f t="shared" ref="F45:F50" si="8">E45/B45*100</f>
         <v>100</v>
       </c>
       <c r="G45" s="4" t="s">
@@ -1507,7 +1507,7 @@
         <v>20</v>
       </c>
       <c r="F46" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>74.07407407</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -1531,7 +1531,7 @@
         <v>9.0</v>
       </c>
       <c r="F47" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>69.23076923</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -1555,7 +1555,7 @@
         <v>29.0</v>
       </c>
       <c r="F48" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>96.66666667</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -1579,7 +1579,7 @@
         <v>14.0</v>
       </c>
       <c r="F49" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>63.63636364</v>
       </c>
       <c r="G49" s="4" t="s">
@@ -1604,7 +1604,7 @@
         <v>85</v>
       </c>
       <c r="F50" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>95.50561798</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -1651,7 +1651,7 @@
         <v>11.0</v>
       </c>
       <c r="F52" s="7">
-        <f t="shared" ref="F52:F57" si="8">E52/B52*100</f>
+        <f t="shared" ref="F52:F57" si="9">E52/B52*100</f>
         <v>100</v>
       </c>
       <c r="G52" s="4" t="s">
@@ -1675,7 +1675,7 @@
         <v>25.0</v>
       </c>
       <c r="F53" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>92.59259259</v>
       </c>
       <c r="G53" s="4" t="s">
@@ -1699,7 +1699,7 @@
         <v>12.0</v>
       </c>
       <c r="F54" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>92.30769231</v>
       </c>
       <c r="G54" s="4" t="s">
@@ -1724,7 +1724,7 @@
         <v>30</v>
       </c>
       <c r="F55" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="G55" s="4" t="s">
@@ -1748,7 +1748,7 @@
         <v>18.0</v>
       </c>
       <c r="F56" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>78.26086957</v>
       </c>
       <c r="G56" s="4" t="s">
@@ -1772,7 +1772,7 @@
         <v>87.0</v>
       </c>
       <c r="F57" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>96.66666667</v>
       </c>
       <c r="G57" s="4" t="s">
@@ -1819,7 +1819,7 @@
         <v>10.0</v>
       </c>
       <c r="F59" s="11">
-        <f t="shared" ref="F59:F61" si="9">E59/B59*100</f>
+        <f t="shared" ref="F59:F61" si="10">E59/B59*100</f>
         <v>90.90909091</v>
       </c>
       <c r="G59" s="4" t="s">
@@ -1843,7 +1843,7 @@
         <v>19.0</v>
       </c>
       <c r="F60" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>70.37037037</v>
       </c>
       <c r="G60" s="4" t="s">
@@ -1867,7 +1867,7 @@
         <v>6.0</v>
       </c>
       <c r="F61" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>46.15384615</v>
       </c>
       <c r="G61" s="4" t="s">
@@ -1987,7 +1987,7 @@
         <v>11.0</v>
       </c>
       <c r="F66" s="11">
-        <f t="shared" ref="F66:F71" si="10">E66/B66*100</f>
+        <f t="shared" ref="F66:F71" si="11">E66/B66*100</f>
         <v>100</v>
       </c>
       <c r="G66" s="4" t="s">
@@ -2011,7 +2011,7 @@
         <v>20.0</v>
       </c>
       <c r="F67" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>74.07407407</v>
       </c>
       <c r="G67" s="4" t="s">
@@ -2035,7 +2035,7 @@
         <v>8.0</v>
       </c>
       <c r="F68" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>61.53846154</v>
       </c>
       <c r="G68" s="4" t="s">
@@ -2060,7 +2060,7 @@
         <v>29</v>
       </c>
       <c r="F69" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>96.66666667</v>
       </c>
       <c r="G69" s="4" t="s">
@@ -2084,7 +2084,7 @@
         <v>14.0</v>
       </c>
       <c r="F70" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>60.86956522</v>
       </c>
       <c r="G70" s="4" t="s">
@@ -2108,7 +2108,7 @@
         <v>86.0</v>
       </c>
       <c r="F71" s="11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>96.62921348</v>
       </c>
       <c r="G71" s="4" t="s">
@@ -2155,7 +2155,7 @@
         <v>11.0</v>
       </c>
       <c r="F73" s="11">
-        <f t="shared" ref="F73:F78" si="11">E73/B73*100</f>
+        <f t="shared" ref="F73:F78" si="12">E73/B73*100</f>
         <v>100</v>
       </c>
       <c r="G73" s="4" t="s">
@@ -2179,7 +2179,7 @@
         <v>22.0</v>
       </c>
       <c r="F74" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>81.48148148</v>
       </c>
       <c r="G74" s="4" t="s">
@@ -2203,7 +2203,7 @@
         <v>8.0</v>
       </c>
       <c r="F75" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>66.66666667</v>
       </c>
       <c r="G75" s="4" t="s">
@@ -2227,7 +2227,7 @@
         <v>28.0</v>
       </c>
       <c r="F76" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>93.33333333</v>
       </c>
       <c r="G76" s="4" t="s">
@@ -2251,7 +2251,7 @@
         <v>17.0</v>
       </c>
       <c r="F77" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>77.27272727</v>
       </c>
       <c r="G77" s="4" t="s">
@@ -2276,7 +2276,7 @@
         <v>85</v>
       </c>
       <c r="F78" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>96.59090909</v>
       </c>
       <c r="G78" s="4" t="s">
@@ -2324,7 +2324,7 @@
         <v>10</v>
       </c>
       <c r="F80" s="11">
-        <f t="shared" ref="F80:F85" si="12">E80/B80*100</f>
+        <f t="shared" ref="F80:F85" si="13">E80/B80*100</f>
         <v>90.90909091</v>
       </c>
       <c r="G80" s="4" t="s">
@@ -2348,7 +2348,7 @@
         <v>24.0</v>
       </c>
       <c r="F81" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>88.88888889</v>
       </c>
       <c r="G81" s="4" t="s">
@@ -2372,7 +2372,7 @@
         <v>7.0</v>
       </c>
       <c r="F82" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>58.33333333</v>
       </c>
       <c r="G82" s="4" t="s">
@@ -2397,7 +2397,7 @@
         <v>28</v>
       </c>
       <c r="F83" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>93.33333333</v>
       </c>
       <c r="G83" s="4" t="s">
@@ -2421,7 +2421,7 @@
         <v>13.0</v>
       </c>
       <c r="F84" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>61.9047619</v>
       </c>
       <c r="G84" s="4" t="s">
@@ -2445,7 +2445,7 @@
         <v>79.0</v>
       </c>
       <c r="F85" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>90.8045977</v>
       </c>
       <c r="G85" s="4" t="s">
@@ -2492,7 +2492,7 @@
         <v>11.0</v>
       </c>
       <c r="F87" s="11">
-        <f t="shared" ref="F87:F92" si="13">E87/B87*100</f>
+        <f t="shared" ref="F87:F92" si="14">E87/B87*100</f>
         <v>100</v>
       </c>
       <c r="G87" s="4" t="s">
@@ -2517,7 +2517,7 @@
         <v>20</v>
       </c>
       <c r="F88" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>74.07407407</v>
       </c>
       <c r="G88" s="4" t="s">
@@ -2541,7 +2541,7 @@
         <v>11.0</v>
       </c>
       <c r="F89" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>84.61538462</v>
       </c>
       <c r="G89" s="4" t="s">
@@ -2565,7 +2565,7 @@
         <v>29.0</v>
       </c>
       <c r="F90" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>96.66666667</v>
       </c>
       <c r="G90" s="4" t="s">
@@ -2589,7 +2589,7 @@
         <v>15.0</v>
       </c>
       <c r="F91" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>68.18181818</v>
       </c>
       <c r="G91" s="4" t="s">
@@ -2614,7 +2614,7 @@
         <v>87</v>
       </c>
       <c r="F92" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>97.75280899</v>
       </c>
       <c r="G92" s="4" t="s">
@@ -2661,7 +2661,7 @@
         <v>11.0</v>
       </c>
       <c r="F94" s="7">
-        <f t="shared" ref="F94:F99" si="14">E94/B94*100</f>
+        <f t="shared" ref="F94:F99" si="15">E94/B94*100</f>
         <v>100</v>
       </c>
       <c r="G94" s="4" t="s">
@@ -2685,7 +2685,7 @@
         <v>26.0</v>
       </c>
       <c r="F95" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>96.2962963</v>
       </c>
       <c r="G95" s="4" t="s">
@@ -2709,7 +2709,7 @@
         <v>12.0</v>
       </c>
       <c r="F96" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>92.30769231</v>
       </c>
       <c r="G96" s="4" t="s">
@@ -2733,7 +2733,7 @@
         <v>30.0</v>
       </c>
       <c r="F97" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
       <c r="G97" s="4" t="s">
@@ -2757,7 +2757,7 @@
         <v>20.0</v>
       </c>
       <c r="F98" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>86.95652174</v>
       </c>
       <c r="G98" s="4" t="s">
@@ -2782,7 +2782,7 @@
         <v>89</v>
       </c>
       <c r="F99" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>98.88888889</v>
       </c>
       <c r="G99" s="4" t="s">
@@ -2829,7 +2829,7 @@
         <v>10.0</v>
       </c>
       <c r="F101" s="7">
-        <f t="shared" ref="F101:F106" si="15">E101/B101*100</f>
+        <f t="shared" ref="F101:F106" si="16">E101/B101*100</f>
         <v>90.90909091</v>
       </c>
       <c r="G101" s="4" t="s">
@@ -2853,7 +2853,7 @@
         <v>22.0</v>
       </c>
       <c r="F102" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>81.48148148</v>
       </c>
       <c r="G102" s="4" t="s">
@@ -2877,7 +2877,7 @@
         <v>7.0</v>
       </c>
       <c r="F103" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>53.84615385</v>
       </c>
       <c r="G103" s="4" t="s">
@@ -2901,7 +2901,7 @@
         <v>27.0</v>
       </c>
       <c r="F104" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>90</v>
       </c>
       <c r="G104" s="4" t="s">
@@ -2925,7 +2925,7 @@
         <v>15.0</v>
       </c>
       <c r="F105" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>65.2173913</v>
       </c>
       <c r="G105" s="4" t="s">
@@ -2950,7 +2950,7 @@
         <v>83</v>
       </c>
       <c r="F106" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>93.25842697</v>
       </c>
       <c r="G106" s="4" t="s">
@@ -3008,7 +3008,7 @@
       <c r="A109" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B109" s="9">
+      <c r="B109" s="14">
         <v>27.0</v>
       </c>
       <c r="C109" s="6" t="s">
@@ -3032,7 +3032,7 @@
       <c r="A110" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B110" s="10">
+      <c r="B110" s="12">
         <v>13.0</v>
       </c>
       <c r="C110" s="6" t="s">
@@ -3045,7 +3045,7 @@
         <v>8.0</v>
       </c>
       <c r="F110" s="7">
-        <f t="shared" ref="F110:F113" si="16">E110/B110*100</f>
+        <f t="shared" ref="F110:F113" si="17">E110/B110*100</f>
         <v>61.53846154</v>
       </c>
       <c r="G110" s="4" t="s">
@@ -3056,7 +3056,7 @@
       <c r="A111" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B111" s="10">
+      <c r="B111" s="12">
         <v>30.0</v>
       </c>
       <c r="C111" s="6" t="s">
@@ -3070,7 +3070,7 @@
         <v>29</v>
       </c>
       <c r="F111" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>96.66666667</v>
       </c>
       <c r="G111" s="4" t="s">
@@ -3081,7 +3081,7 @@
       <c r="A112" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B112" s="10">
+      <c r="B112" s="12">
         <v>23.0</v>
       </c>
       <c r="C112" s="8" t="s">
@@ -3094,7 +3094,7 @@
         <v>14.0</v>
       </c>
       <c r="F112" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>60.86956522</v>
       </c>
       <c r="G112" s="4" t="s">
@@ -3105,7 +3105,7 @@
       <c r="A113" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B113" s="10">
+      <c r="B113" s="12">
         <v>89.0</v>
       </c>
       <c r="C113" s="6" t="s">
@@ -3119,7 +3119,7 @@
         <v>86</v>
       </c>
       <c r="F113" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>96.62921348</v>
       </c>
       <c r="G113" s="4" t="s">
@@ -3166,7 +3166,7 @@
         <v>11.0</v>
       </c>
       <c r="F115" s="7">
-        <f t="shared" ref="F115:F120" si="17">E115/B115*100</f>
+        <f t="shared" ref="F115:F120" si="18">E115/B115*100</f>
         <v>100</v>
       </c>
       <c r="G115" s="4" t="s">
@@ -3190,7 +3190,7 @@
         <v>25.0</v>
       </c>
       <c r="F116" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>92.59259259</v>
       </c>
       <c r="G116" s="4" t="s">
@@ -3214,7 +3214,7 @@
         <v>8.0</v>
       </c>
       <c r="F117" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>66.66666667</v>
       </c>
       <c r="G117" s="4" t="s">
@@ -3238,7 +3238,7 @@
         <v>28.0</v>
       </c>
       <c r="F118" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>93.33333333</v>
       </c>
       <c r="G118" s="4" t="s">
@@ -3262,7 +3262,7 @@
         <v>17.0</v>
       </c>
       <c r="F119" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>77.27272727</v>
       </c>
       <c r="G119" s="4" t="s">
@@ -3286,7 +3286,7 @@
         <v>85.0</v>
       </c>
       <c r="F120" s="7">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>96.59090909</v>
       </c>
       <c r="G120" s="4" t="s">
@@ -3334,7 +3334,7 @@
         <v>11</v>
       </c>
       <c r="F122" s="7">
-        <f t="shared" ref="F122:F127" si="18">E122/B122*100</f>
+        <f t="shared" ref="F122:F127" si="19">E122/B122*100</f>
         <v>100</v>
       </c>
       <c r="G122" s="4" t="s">
@@ -3358,7 +3358,7 @@
         <v>25.0</v>
       </c>
       <c r="F123" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>92.59259259</v>
       </c>
       <c r="G123" s="4" t="s">
@@ -3382,7 +3382,7 @@
         <v>7.0</v>
       </c>
       <c r="F124" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>58.33333333</v>
       </c>
       <c r="G124" s="4" t="s">
@@ -3406,7 +3406,7 @@
         <v>28.0</v>
       </c>
       <c r="F125" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>93.33333333</v>
       </c>
       <c r="G125" s="4" t="s">
@@ -3430,7 +3430,7 @@
         <v>13.0</v>
       </c>
       <c r="F126" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>61.9047619</v>
       </c>
       <c r="G126" s="4" t="s">
@@ -3454,7 +3454,7 @@
         <v>79.0</v>
       </c>
       <c r="F127" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>90.8045977</v>
       </c>
       <c r="G127" s="4" t="s">

</xml_diff>